<commit_message>
WI2:IRCTC.xlsx completed scenario, updated ECP and test cases
</commit_message>
<xml_diff>
--- a/IRCTC.xlsx
+++ b/IRCTC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubhasmita_roy\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="8_{01087A6F-76CB-48D2-8ED1-F5527F7563D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DE8D8ED-4858-46A7-8CC6-58876D4FE431}"/>
+  <xr:revisionPtr revIDLastSave="486" documentId="8_{01087A6F-76CB-48D2-8ED1-F5527F7563D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1637A2B1-8277-4B51-930E-E12900BBEA72}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{0FAB5BBC-C930-4DD0-8EFE-50F36BC1F008}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="3" xr2:uid="{0FAB5BBC-C930-4DD0-8EFE-50F36BC1F008}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Required" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
   <si>
     <r>
       <t>·</t>
@@ -179,6 +179,12 @@
     <t>User must be on the ticket booking page</t>
   </si>
   <si>
+    <t>To test if user can book ticket without completing payment</t>
+  </si>
+  <si>
+    <t>To test if user can book the ticket without entering the verification CAPTCHA.</t>
+  </si>
+  <si>
     <t>Sc_04</t>
   </si>
   <si>
@@ -197,7 +203,7 @@
     <t>The PNR number must be active and authenticated</t>
   </si>
   <si>
-    <t>To check the running tatus of the train using PNR number</t>
+    <t>To check the running status of the train using PNR number</t>
   </si>
   <si>
     <t>To check the passenger details using PNR number</t>
@@ -263,9 +269,96 @@
     <t>Sc_01Tc_01</t>
   </si>
   <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>Enter correct user id</t>
+  </si>
+  <si>
+    <t>User id should be displayed</t>
+  </si>
+  <si>
+    <t>User id is displayed</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>Enter correct password</t>
+  </si>
+  <si>
+    <t>Password should be hidden</t>
+  </si>
+  <si>
+    <t>Enter correct CAPTCHA</t>
+  </si>
+  <si>
     <t>Sc_01Tc_02</t>
   </si>
   <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>Enter incorrect password</t>
+  </si>
+  <si>
+    <t>Enter incorrect CAPTCHA</t>
+  </si>
+  <si>
+    <t>Sc_01Tc_03</t>
+  </si>
+  <si>
+    <t>Leave password field empty</t>
+  </si>
+  <si>
+    <t>Sc_02Tc_01</t>
+  </si>
+  <si>
+    <t>Sc_02Tc_02</t>
+  </si>
+  <si>
+    <t>Sc_02Tc_03</t>
+  </si>
+  <si>
+    <t>Sc_02Tc_04</t>
+  </si>
+  <si>
+    <t>Sc_03Tc_01</t>
+  </si>
+  <si>
+    <t>Sc_03Tc_02</t>
+  </si>
+  <si>
+    <t>Sc_03Tc_03</t>
+  </si>
+  <si>
+    <t>Sc_03Tc_04</t>
+  </si>
+  <si>
+    <t>Sc_04Tc_01</t>
+  </si>
+  <si>
+    <t>Sc_04Tc_02</t>
+  </si>
+  <si>
+    <t>Sc_04Tc_03</t>
+  </si>
+  <si>
+    <t>Sc_04Tc_04</t>
+  </si>
+  <si>
+    <t>Sc_05Tc_01</t>
+  </si>
+  <si>
+    <t>Sc_05Tc_02</t>
+  </si>
+  <si>
+    <t>Sc_05Tc_03</t>
+  </si>
+  <si>
     <t>Product Name</t>
   </si>
   <si>
@@ -329,7 +422,7 @@
     <t>2 years</t>
   </si>
   <si>
-    <t xml:space="preserve">No booking </t>
+    <t>Booking Rejected</t>
   </si>
   <si>
     <t>fail</t>
@@ -344,37 +437,85 @@
     <t>25 years</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>60 above</t>
+    <t>Booking Confirmed</t>
+  </si>
+  <si>
+    <t>60 and above</t>
+  </si>
+  <si>
+    <t>69 YEARS</t>
   </si>
   <si>
     <t>Checking if railaway employee + fam or not</t>
   </si>
   <si>
+    <t>If Employee</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>If Not Employee</t>
+  </si>
+  <si>
+    <t>If Employee Family</t>
+  </si>
+  <si>
+    <t>Employee Family</t>
+  </si>
+  <si>
+    <t>If Not Employee Family</t>
+  </si>
+  <si>
+    <t>Tatkaal Window opens 1 day before- 10 am AC 11am Non AC</t>
+  </si>
+  <si>
+    <t>12:15 am to 9:59 am</t>
+  </si>
+  <si>
+    <t>Window Closes</t>
+  </si>
+  <si>
+    <t>10:00 am onwards (AC)</t>
+  </si>
+  <si>
+    <t>window opened</t>
+  </si>
+  <si>
+    <t>11:00 am onwards (Non-Ac)</t>
+  </si>
+  <si>
+    <t>BVA</t>
+  </si>
+  <si>
+    <t>Valid min -1 = 4</t>
+  </si>
+  <si>
+    <t>min =5</t>
+  </si>
+  <si>
+    <t>min+1=6</t>
+  </si>
+  <si>
+    <t>max-1 = 59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max = 60 </t>
+  </si>
+  <si>
+    <t>max+1=61</t>
+  </si>
+  <si>
     <t>tatkaal Window opens 1 day before- 10 am AC 11am Non AC</t>
   </si>
   <si>
-    <t>BVA</t>
-  </si>
-  <si>
-    <t>min -1 = 4</t>
-  </si>
-  <si>
-    <t>min =5</t>
-  </si>
-  <si>
-    <t>min+1=6</t>
-  </si>
-  <si>
-    <t>max-1 = 59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max = 60 </t>
-  </si>
-  <si>
-    <t>max+1=61</t>
+    <t>Valid min-1= 9:59 am</t>
+  </si>
+  <si>
+    <t>min=10:00 am</t>
+  </si>
+  <si>
+    <t>min+1=10:01 am</t>
   </si>
   <si>
     <t xml:space="preserve">State </t>
@@ -402,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +621,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -501,7 +648,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -543,21 +690,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -635,11 +767,188 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -647,15 +956,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -665,33 +973,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -701,7 +992,86 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1061,249 +1431,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340DA108-7BA2-4179-BE7B-470305B912CE}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="23" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="23" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30.75">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="47.25" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="12"/>
+      <c r="D3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34.5" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="D4" s="12" t="s">
+      <c r="A4" s="12"/>
+      <c r="D4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A5" s="13"/>
+      <c r="A5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A6" s="13"/>
+      <c r="A6" s="12"/>
     </row>
     <row r="7" spans="1:5" ht="15"/>
     <row r="8" spans="1:5" ht="45.75">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" customHeight="1">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30.75">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" ht="15"/>
     <row r="14" spans="1:5" ht="15"/>
     <row r="15" spans="1:5" ht="60.75">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30.75">
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30.75">
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15"/>
-    <row r="19" spans="1:5" ht="45.75">
-      <c r="A19" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="12" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="30.75">
+      <c r="E18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="12" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="15"/>
+    <row r="20" spans="1:5" ht="45.75">
+      <c r="A20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="B20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30.75">
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30.75">
+      <c r="D21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30.75">
-      <c r="D21" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15">
-      <c r="D22" s="13"/>
-      <c r="E22" s="12" t="s">
+    <row r="22" spans="1:5" ht="30.75">
+      <c r="D22" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="E22" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15">
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" ht="30.75">
-      <c r="A24" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="12" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="14" t="s">
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" ht="30.75">
+      <c r="A25" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30.75">
-      <c r="D25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>42</v>
+      <c r="E25" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30.75">
       <c r="D26" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
-      <c r="D27" s="12" t="s">
+    <row r="27" spans="1:5" ht="30.75">
+      <c r="D27" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="E27" s="20" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="15">
-      <c r="D28" s="12" t="s">
-        <v>46</v>
+      <c r="D28" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15">
+      <c r="D29" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1698,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18"/>
+      <c r="A1" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1329,17 +1707,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C2FA82-C499-4B75-9180-8811DCDC06DD}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
@@ -1348,59 +1728,360 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="45.75">
-      <c r="A2" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="L1" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="48" customHeight="1">
+      <c r="A2" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="45.75">
-      <c r="A4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="C2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="39">
+        <v>1</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="37"/>
+      <c r="L2" s="48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30.75">
+      <c r="A3" s="46"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35">
+        <v>2</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="49"/>
+    </row>
+    <row r="4" spans="1:12" ht="30.75">
+      <c r="A4" s="47"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41">
+        <v>3</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="50"/>
+    </row>
+    <row r="6" spans="1:12" ht="45.75">
+      <c r="A6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="21"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30.75">
+      <c r="A8" s="21"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60.75">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30.75">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45.75">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30.75">
+      <c r="B16" s="12"/>
+      <c r="C16" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" ht="137.25">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30.75">
+      <c r="B20" s="12"/>
+      <c r="C20" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="76.5">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="60.75">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="76.5">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60.75">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="76.5">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="76.5">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="60.75">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="76.5">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="60.75">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="60.75">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="60.75">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="76.5">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="60.75">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1423,45 +2104,45 @@
     <col min="13" max="13" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="12" customFormat="1" ht="45.75">
-      <c r="A1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>71</v>
+    <row r="1" spans="1:13" s="11" customFormat="1" ht="45.75">
+      <c r="A1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1471,208 +2152,332 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B60BB-59B2-4C78-8645-AB541379F354}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="13" style="24" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>55</v>
+      <c r="A1" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
-        <v>82</v>
+      <c r="A2" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="22"/>
-      <c r="B3" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
-        <v>86</v>
+      <c r="A3" s="26"/>
+      <c r="B3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20" t="s">
-        <v>86</v>
+      <c r="A4" s="26"/>
+      <c r="B4" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="A5" s="26"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="26"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="23" t="s">
-        <v>88</v>
+      <c r="A7" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="23"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="23"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="23"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="23"/>
+      <c r="A11" s="27"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="23" t="s">
-        <v>89</v>
+      <c r="A12" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="23"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="23"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="23"/>
+      <c r="A15" s="27"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="23"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="23"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="23"/>
-      <c r="B20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="23"/>
-      <c r="B21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="23"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="23"/>
-      <c r="B23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="23"/>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="23"/>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="23"/>
+      <c r="A16" s="27"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="27"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="27"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="27"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="27"/>
+      <c r="B30" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="27"/>
+      <c r="B31" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="27"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="27"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="A19:A26"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1692,17 +2497,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>100</v>
+      <c r="A1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1721,14 +2526,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>103</v>
+      <c r="A1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1737,9 +2542,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1875,16 +2683,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E269AE-C7DC-46B2-AEC9-FF65149B2B13}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B028AD-C993-4B97-948A-E65FE838CF9E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1892,5 +2697,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B028AD-C993-4B97-948A-E65FE838CF9E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E269AE-C7DC-46B2-AEC9-FF65149B2B13}"/>
 </file>
</xml_diff>